<commit_message>
Fix eliminacion de registros previos Excel
</commit_message>
<xml_diff>
--- a/WebApp/Files/cargaDataBusccadorAndino.xlsx
+++ b/WebApp/Files/cargaDataBusccadorAndino.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arupo\Documents\dotNet\Buscador\WebApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339D1ED8-1D87-454A-BB80-320AE8E6391E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE649B96-B21D-4B1E-B3AC-1A03C358BFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{227A6549-022C-499C-9D9D-BE9574C66532}"/>
   </bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AE43D8-A90F-431E-8B7E-EF5425F0292A}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +661,7 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>45448</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>45448</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>45448</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>45448</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2">
         <v>45448</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>45448</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>45448</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>45448</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>45448</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>45448</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>45448</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>45448</v>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2">
         <v>45448</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>45448</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B16" s="2">
         <v>45448</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B17" s="2">
         <v>45448</v>
@@ -1653,7 +1653,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B18" s="2">
         <v>45448</v>

</xml_diff>